<commit_message>
Almost done with Lab 3
</commit_message>
<xml_diff>
--- a/Lab #3 - Hall Effect/Data/HallData.xlsx
+++ b/Lab #3 - Hall Effect/Data/HallData.xlsx
@@ -8,6 +8,7 @@
     <sheet state="visible" name="Part 2" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Part 3" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Part 4" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Part 5" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>I_p [mA]</t>
   </si>
@@ -56,7 +57,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -74,6 +75,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -113,6 +118,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,11 +199,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1686003866"/>
-        <c:axId val="1626821882"/>
+        <c:axId val="368924756"/>
+        <c:axId val="2145131651"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1686003866"/>
+        <c:axId val="368924756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -244,10 +255,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1626821882"/>
+        <c:crossAx val="2145131651"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1626821882"/>
+        <c:axId val="2145131651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -322,7 +333,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1686003866"/>
+        <c:crossAx val="368924756"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -414,11 +425,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1722807174"/>
-        <c:axId val="203618931"/>
+        <c:axId val="1066974165"/>
+        <c:axId val="1230171104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1722807174"/>
+        <c:axId val="1066974165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -470,10 +481,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203618931"/>
+        <c:crossAx val="1230171104"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="203618931"/>
+        <c:axId val="1230171104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +559,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1722807174"/>
+        <c:crossAx val="1066974165"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -640,11 +651,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42222982"/>
-        <c:axId val="1219767805"/>
+        <c:axId val="1010997465"/>
+        <c:axId val="1583084041"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42222982"/>
+        <c:axId val="1010997465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="310.0"/>
@@ -697,10 +708,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1219767805"/>
+        <c:crossAx val="1583084041"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1219767805"/>
+        <c:axId val="1583084041"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +786,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42222982"/>
+        <c:crossAx val="1010997465"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -867,11 +878,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="328040969"/>
-        <c:axId val="846395181"/>
+        <c:axId val="690825013"/>
+        <c:axId val="1797865505"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="328040969"/>
+        <c:axId val="690825013"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="305.0"/>
@@ -924,10 +935,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="846395181"/>
+        <c:crossAx val="1797865505"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="846395181"/>
+        <c:axId val="1797865505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.34"/>
@@ -1003,7 +1014,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="328040969"/>
+        <c:crossAx val="690825013"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1053,7 +1064,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>U_P [V] vs. B [mT]</a:t>
+              <a:t>U_P [V] vs. T [deg C]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1064,14 +1075,45 @@
       <c:layout/>
       <c:lineChart>
         <c:varyColors val="0"/>
-        <c:axId val="1096365696"/>
-        <c:axId val="458554193"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Part 4'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Part 4'!$A$2:$A$31</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Part 4'!$B$2:$B$31</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1194432337"/>
+        <c:axId val="1823209022"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1096365696"/>
+        <c:axId val="1194432337"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="305.0"/>
+          <c:max val="150.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1096,7 +1138,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>B [mT]</a:t>
+                  <a:t>T [deg C]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1121,22 +1163,312 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458554193"/>
+        <c:crossAx val="1823209022"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="458554193"/>
+        <c:axId val="1823209022"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>U_P [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1194432337"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>U_H [mV] vs. T [deg C]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Part 5'!$B$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Part 5'!$A$2:$A$31</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Part 5'!$B$2:$B$31</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1562298286"/>
+        <c:axId val="176541220"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1562298286"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>T [deg C]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="176541220"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="176541220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>U_H [mV]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
+          <a:ln/>
         </c:spPr>
-        <c:crossAx val="1096365696"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1562298286"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1295,6 +1627,36 @@
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2280,113 +2642,542 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="B2" s="2"/>
+        <v>30.0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.3725</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="B3" s="2"/>
+        <f t="shared" ref="A3:A15" si="1">A2+5</f>
+        <v>35</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.414</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
-        <f t="shared" ref="A4:A17" si="1">A3+20</f>
+      <c r="A4" s="2">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="2">
+        <v>1.4661</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1.5112</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.5983</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B8" s="2">
+        <v>1.6309</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.6569</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.6675</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1.6553</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.6262</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.5661</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.4837</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.3674</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1.2538</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>105.0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1.1087</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>110.0</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.9867</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>115.0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.8602</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <f>120</f>
+        <v>120</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.7574</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <f t="shared" ref="A21:A30" si="2">A20+2</f>
+        <v>122</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.715</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.6813</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.6339</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.5965</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.5642</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.5379</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.5093</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="B28" s="8">
+        <v>0.4844</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.4609</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.4437</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>-114.07</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <f t="shared" ref="A3:A15" si="1">A2+5</f>
+        <v>35</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-115.6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B4" s="2">
+        <v>-118.05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="B5" s="7">
+        <v>-119.92</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-122.26</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-123.24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-124.55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-124.71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-123.73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-121.7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <f t="shared" si="1"/>
+      <c r="B12" s="2">
+        <v>-116.98</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="B13" s="2">
+        <v>-111.91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B14" s="2">
+        <v>-100.97</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="B15" s="2">
+        <v>-93.39</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>100.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>-82.88</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>105.0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>-72.64</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>110.0</v>
+      </c>
+      <c r="B18" s="9">
+        <v>-61.11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>115.0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-53.2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3">
+        <f>120</f>
         <v>120</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3">
-        <f t="shared" si="1"/>
+      <c r="B20" s="9">
+        <v>-43.58</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3">
+        <f t="shared" ref="A21:A30" si="2">A20+2</f>
+        <v>122</v>
+      </c>
+      <c r="B21" s="8">
+        <v>-40.93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="B22" s="8">
+        <v>-37.4</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="B23" s="8">
+        <v>-35.3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="B24" s="8">
+        <v>-33.37</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="B25" s="8">
+        <v>-30.81</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="B26" s="8">
+        <v>-29.29</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="B27" s="8">
+        <v>-27.22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="B28" s="8">
+        <v>-25.39</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="B29" s="8">
+        <v>-23.76</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3">
+        <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="3">
-        <f t="shared" si="1"/>
-        <v>160</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3">
-        <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3">
-        <f t="shared" si="1"/>
-        <v>200</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3">
-        <f t="shared" si="1"/>
-        <v>220</v>
-      </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
-        <v>240</v>
-      </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="3">
-        <f t="shared" si="1"/>
-        <v>260</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="3">
-        <f t="shared" si="1"/>
-        <v>280</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="3">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="B17" s="2"/>
+      <c r="B30" s="8">
+        <v>-22.77</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2"/>
+      <c r="B31" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>